<commit_message>
Version 24/10/24 add Enum Class
</commit_message>
<xml_diff>
--- a/Class structure.xlsx
+++ b/Class structure.xlsx
@@ -35,9 +35,6 @@
     <t>Комментарий руководителя проекта</t>
   </si>
   <si>
-    <t>Файл</t>
-  </si>
-  <si>
     <t>Записывает в файл Запись</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>StringPattern - Обработка строки - Шаблон</t>
+  </si>
+  <si>
+    <t>FileService</t>
   </si>
 </sst>
 </file>
@@ -587,7 +587,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,155 +614,155 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="8" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
         <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>21</v>
-      </c>
-      <c r="C23" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>